<commit_message>
Modified calibration.xlsx file to include short range sensors.
</commit_message>
<xml_diff>
--- a/Calibration.xlsx
+++ b/Calibration.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Distance (mm) </t>
   </si>
@@ -35,7 +35,19 @@
     <t>sensor Lr 2</t>
   </si>
   <si>
-    <t>Average</t>
+    <t>S1-M</t>
+  </si>
+  <si>
+    <t>S2-M</t>
+  </si>
+  <si>
+    <t>Average (long range)</t>
+  </si>
+  <si>
+    <t>Average (short range)</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -163,14 +175,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average (long range)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -193,7 +216,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$35</c:f>
               <c:numCache>
@@ -303,8 +326,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$35</c:f>
               <c:numCache>
@@ -414,7 +437,230 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average (short range)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>675</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>775</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>850</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>672.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>578.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>485.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>285.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>282.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>197.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>185.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>157.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>151.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>133.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>110.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -425,18 +671,72 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="226990224"/>
-        <c:axId val="227997080"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="226990224"/>
+        <c:axId val="180489448"/>
+        <c:axId val="180489840"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="180489448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Distance (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -446,8 +746,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -474,15 +774,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227997080"/>
+        <c:crossAx val="180489840"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="227997080"/>
+        <c:axId val="180489840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -502,14 +799,76 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Sensor readings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -533,9 +892,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226990224"/>
+        <c:crossAx val="180489448"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -545,8 +904,40 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -623,7 +1014,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -650,8 +1041,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -752,7 +1143,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -784,10 +1175,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -827,22 +1218,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -947,8 +1339,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1080,19 +1472,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1106,6 +1499,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1129,20 +1533,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1423,10 +1827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1840,7 @@
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1447,10 +1851,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>25</v>
       </c>
@@ -1464,8 +1880,22 @@
         <f>AVERAGE(B2:C2)</f>
         <v>312.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>B2-C2</f>
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>605</v>
+      </c>
+      <c r="G2">
+        <v>575</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(F2:G2)</f>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -1479,8 +1909,22 @@
         <f t="shared" ref="D3:D35" si="0">AVERAGE(B3:C3)</f>
         <v>359</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E35" si="1">B3-C3</f>
+        <v>-8</v>
+      </c>
+      <c r="F3">
+        <v>680</v>
+      </c>
+      <c r="G3">
+        <v>665</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H22" si="2">AVERAGE(F3:G3)</f>
+        <v>672.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>75</v>
       </c>
@@ -1494,8 +1938,22 @@
         <f t="shared" si="0"/>
         <v>386.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>580</v>
+      </c>
+      <c r="G4">
+        <v>577</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>578.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
@@ -1509,8 +1967,22 @@
         <f t="shared" si="0"/>
         <v>491</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>461</v>
+      </c>
+      <c r="G5">
+        <v>510</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>485.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>125</v>
       </c>
@@ -1524,8 +1996,22 @@
         <f t="shared" si="0"/>
         <v>571</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
+      <c r="F6">
+        <v>365</v>
+      </c>
+      <c r="G6">
+        <v>315</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>150</v>
       </c>
@@ -1539,8 +2025,22 @@
         <f t="shared" si="0"/>
         <v>568</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>-16</v>
+      </c>
+      <c r="F7">
+        <v>306</v>
+      </c>
+      <c r="G7">
+        <v>265</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>285.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>175</v>
       </c>
@@ -1554,8 +2054,22 @@
         <f t="shared" si="0"/>
         <v>544.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>-21</v>
+      </c>
+      <c r="F8">
+        <v>275</v>
+      </c>
+      <c r="G8">
+        <v>290</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>282.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>200</v>
       </c>
@@ -1569,8 +2083,22 @@
         <f t="shared" si="0"/>
         <v>521</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>-16</v>
+      </c>
+      <c r="F9">
+        <v>250</v>
+      </c>
+      <c r="G9">
+        <v>256</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>225</v>
       </c>
@@ -1584,8 +2112,22 @@
         <f t="shared" si="0"/>
         <v>491.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>-13</v>
+      </c>
+      <c r="F10">
+        <v>216</v>
+      </c>
+      <c r="G10">
+        <v>222</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>250</v>
       </c>
@@ -1599,8 +2141,22 @@
         <f t="shared" si="0"/>
         <v>458.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>-7</v>
+      </c>
+      <c r="F11">
+        <v>199</v>
+      </c>
+      <c r="G11">
+        <v>196</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>197.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>275</v>
       </c>
@@ -1614,8 +2170,22 @@
         <f t="shared" si="0"/>
         <v>433</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="F12">
+        <v>185</v>
+      </c>
+      <c r="G12">
+        <v>186</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>185.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>300</v>
       </c>
@@ -1629,8 +2199,22 @@
         <f t="shared" si="0"/>
         <v>407.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>165</v>
+      </c>
+      <c r="G13">
+        <v>169</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>325</v>
       </c>
@@ -1644,8 +2228,22 @@
         <f t="shared" si="0"/>
         <v>376.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>155</v>
+      </c>
+      <c r="G14">
+        <v>160</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>350</v>
       </c>
@@ -1659,8 +2257,22 @@
         <f t="shared" si="0"/>
         <v>354</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>151</v>
+      </c>
+      <c r="G15">
+        <v>152</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>151.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>375</v>
       </c>
@@ -1674,8 +2286,22 @@
         <f t="shared" si="0"/>
         <v>330.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>132</v>
+      </c>
+      <c r="G16">
+        <v>135</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>133.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>400</v>
       </c>
@@ -1689,8 +2315,22 @@
         <f t="shared" si="0"/>
         <v>314</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>127</v>
+      </c>
+      <c r="G17">
+        <v>131</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>425</v>
       </c>
@@ -1704,8 +2344,22 @@
         <f t="shared" si="0"/>
         <v>294.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="F18">
+        <v>126</v>
+      </c>
+      <c r="G18">
+        <v>120</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>450</v>
       </c>
@@ -1719,8 +2373,22 @@
         <f t="shared" si="0"/>
         <v>279</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="F19">
+        <v>115</v>
+      </c>
+      <c r="G19">
+        <v>117</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>475</v>
       </c>
@@ -1734,8 +2402,22 @@
         <f t="shared" si="0"/>
         <v>266</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>115</v>
+      </c>
+      <c r="G20">
+        <v>106</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>500</v>
       </c>
@@ -1749,8 +2431,22 @@
         <f t="shared" si="0"/>
         <v>253</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+      <c r="G21">
+        <v>102</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>525</v>
       </c>
@@ -1764,8 +2460,22 @@
         <f t="shared" si="0"/>
         <v>242</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>102</v>
+      </c>
+      <c r="G22">
+        <v>98</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>550</v>
       </c>
@@ -1779,8 +2489,12 @@
         <f t="shared" si="0"/>
         <v>230.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>575</v>
       </c>
@@ -1794,8 +2508,12 @@
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>600</v>
       </c>
@@ -1809,8 +2527,12 @@
         <f t="shared" si="0"/>
         <v>210.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>625</v>
       </c>
@@ -1824,8 +2546,12 @@
         <f t="shared" si="0"/>
         <v>202.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>650</v>
       </c>
@@ -1839,8 +2565,12 @@
         <f t="shared" si="0"/>
         <v>198.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>675</v>
       </c>
@@ -1854,8 +2584,12 @@
         <f t="shared" si="0"/>
         <v>186.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>700</v>
       </c>
@@ -1869,8 +2603,12 @@
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>725</v>
       </c>
@@ -1884,8 +2622,12 @@
         <f t="shared" si="0"/>
         <v>175.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>750</v>
       </c>
@@ -1899,8 +2641,12 @@
         <f t="shared" si="0"/>
         <v>169.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>775</v>
       </c>
@@ -1914,8 +2660,12 @@
         <f t="shared" si="0"/>
         <v>163.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>800</v>
       </c>
@@ -1929,8 +2679,12 @@
         <f t="shared" si="0"/>
         <v>159.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>825</v>
       </c>
@@ -1944,8 +2698,12 @@
         <f t="shared" si="0"/>
         <v>156.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>850</v>
       </c>
@@ -1958,6 +2716,10 @@
       <c r="D35">
         <f t="shared" si="0"/>
         <v>151.5</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>